<commit_message>
Nano code timing optimisation
</commit_message>
<xml_diff>
--- a/ArduinoCode/PGN OG3D.xlsx
+++ b/ArduinoCode/PGN OG3D.xlsx
@@ -899,10 +899,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="9.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="6" style="4" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="8" style="4" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="5" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="5" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="6" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="5" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="6" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>